<commit_message>
Fixed missing criterion bug, re-ran on all test cases
</commit_message>
<xml_diff>
--- a/S2022_Tests/ASS_00_Dim_Testing/KEY/LEGO_BRICK_dnobes_F2021_SOLUTION/ExcelExtract.xlsx
+++ b/S2022_Tests/ASS_00_Dim_Testing/KEY/LEGO_BRICK_dnobes_F2021_SOLUTION/ExcelExtract.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zacha\OneDrive\Desktop\Ualberta Summer 2022 Co-op\SolidWorks\AutoMARK\AutoMARK_V6\S2022_Tests\ASS_00_Dim_Testing\KEY\LEGO_BRICK_dnobes_F2021_SOLUTION\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3E28CFA5-D873-4ABB-B513-BBF753C80B8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{86844B95-ECF8-4D28-B25F-B9F0A2DC378B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="953" yWindow="2847" windowWidth="13120" windowHeight="7660" xr2:uid="{66D94982-A078-4B36-8D5B-7EAD2FA2A3D5}"/>
+    <workbookView xWindow="953" yWindow="2847" windowWidth="13120" windowHeight="7660" xr2:uid="{371E8DEF-BF7F-4969-8C50-AE00E7D4F83E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1403,7 +1403,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB6504D2-09AD-49BA-8DB7-F747CA62E837}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{520A6CF1-83A1-4D95-A6BB-0EFA5D7750FB}">
   <dimension ref="A1:AS125"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
Fixed arrowside issue: assumption that dims only have one arrowhead was wrong, changes to macros and criterionDimensionArrowSide.m, re-ran on all tests
</commit_message>
<xml_diff>
--- a/S2022_Tests/ASS_00_Dim_Testing/KEY/LEGO_BRICK_dnobes_F2021_SOLUTION/ExcelExtract.xlsx
+++ b/S2022_Tests/ASS_00_Dim_Testing/KEY/LEGO_BRICK_dnobes_F2021_SOLUTION/ExcelExtract.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zacha\OneDrive\Desktop\Ualberta Summer 2022 Co-op\SolidWorks\AutoMARK\AutoMARK_V6\S2022_Tests\ASS_00_Dim_Testing\KEY\LEGO_BRICK_dnobes_F2021_SOLUTION\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{86844B95-ECF8-4D28-B25F-B9F0A2DC378B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5CC66BEC-FFD1-41FE-9714-88FB848CA926}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="953" yWindow="2847" windowWidth="13120" windowHeight="7660" xr2:uid="{371E8DEF-BF7F-4969-8C50-AE00E7D4F83E}"/>
+    <workbookView xWindow="13" yWindow="4847" windowWidth="24860" windowHeight="7800" xr2:uid="{2B4D6B18-1690-4593-9CF0-676F9A12F766}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1403,7 +1403,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{520A6CF1-83A1-4D95-A6BB-0EFA5D7750FB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D6B6D18-DC17-453F-82E6-F90D959DFF05}">
   <dimension ref="A1:AS125"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -6532,7 +6532,7 @@
         <v>2</v>
       </c>
       <c r="F74">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G74">
         <v>1</v>
@@ -6645,7 +6645,7 @@
         <v>2</v>
       </c>
       <c r="F75">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G75">
         <v>1</v>
@@ -8553,7 +8553,7 @@
         <v>2</v>
       </c>
       <c r="F96">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G96">
         <v>1</v>

</xml_diff>

<commit_message>
Fixed bug in template GUI and marking sheet mass
</commit_message>
<xml_diff>
--- a/S2022_Tests/ASS_00_Dim_Testing/KEY/LEGO_BRICK_dnobes_F2021_SOLUTION/ExcelExtract.xlsx
+++ b/S2022_Tests/ASS_00_Dim_Testing/KEY/LEGO_BRICK_dnobes_F2021_SOLUTION/ExcelExtract.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zacha\OneDrive\Desktop\Ualberta Summer 2022 Co-op\SolidWorks\AutoMARK\AutoMARK_V6\S2022_Tests\ASS_00_Dim_Testing\KEY\LEGO_BRICK_dnobes_F2021_SOLUTION\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5CC66BEC-FFD1-41FE-9714-88FB848CA926}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5F497C1F-73AA-4D3E-8C9E-DFF26D10E5FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13" yWindow="4847" windowWidth="24860" windowHeight="7800" xr2:uid="{2B4D6B18-1690-4593-9CF0-676F9A12F766}"/>
+    <workbookView xWindow="13" yWindow="4847" windowWidth="24860" windowHeight="7800" xr2:uid="{0F65CEE3-5FFE-4C10-A000-141338F9038A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1403,7 +1403,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D6B6D18-DC17-453F-82E6-F90D959DFF05}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B24D7D7-B6F5-4A04-A44C-91FF867AA9EE}">
   <dimension ref="A1:AS125"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -6616,13 +6616,13 @@
         <v>0</v>
       </c>
       <c r="AP74">
-        <v>4.5280113207547074E-2</v>
+        <v>4.5280113207547115E-2</v>
       </c>
       <c r="AQ74">
         <v>0.13875716981132069</v>
       </c>
       <c r="AR74">
-        <v>4.5280113207547074E-2</v>
+        <v>4.5280113207547115E-2</v>
       </c>
       <c r="AS74">
         <v>0.10125716981132069</v>
@@ -6729,13 +6729,13 @@
         <v>0</v>
       </c>
       <c r="AP75">
-        <v>3.3280113207547063E-2</v>
+        <v>3.3280113207547105E-2</v>
       </c>
       <c r="AQ75">
         <v>0.1512571698113207</v>
       </c>
       <c r="AR75">
-        <v>3.3280113207547063E-2</v>
+        <v>3.3280113207547105E-2</v>
       </c>
       <c r="AS75">
         <v>0.10125716981132069</v>
@@ -6955,16 +6955,16 @@
         <v>0</v>
       </c>
       <c r="AP77">
-        <v>0.19568968234456149</v>
+        <v>0.19568968234456152</v>
       </c>
       <c r="AQ77">
         <v>0.10125716981132069</v>
       </c>
       <c r="AR77">
-        <v>0.16255547525085495</v>
+        <v>0.16255547525085492</v>
       </c>
       <c r="AS77">
-        <v>0.11498180776801278</v>
+        <v>0.11498180776801281</v>
       </c>
     </row>
     <row r="78" spans="1:45" s="4" customFormat="1" x14ac:dyDescent="0.5">
@@ -7700,13 +7700,13 @@
         <v>0.17378011320754708</v>
       </c>
       <c r="AQ88">
-        <v>0.25113373584905668</v>
+        <v>0.25113373584905663</v>
       </c>
       <c r="AR88">
         <v>6.1280113207547067E-2</v>
       </c>
       <c r="AS88">
-        <v>0.25113373584905657</v>
+        <v>0.25113373584905652</v>
       </c>
     </row>
     <row r="89" spans="1:45" x14ac:dyDescent="0.5">
@@ -7816,16 +7816,16 @@
         <v>0</v>
       </c>
       <c r="AP89">
-        <v>8.5442771981199872E-2</v>
+        <v>8.5442771981199886E-2</v>
       </c>
       <c r="AQ89">
-        <v>0.20125873584905662</v>
+        <v>0.2012587358490566</v>
       </c>
       <c r="AR89">
-        <v>7.4617454433894337E-2</v>
+        <v>7.4617454433894351E-2</v>
       </c>
       <c r="AS89">
-        <v>0.20750873584905655</v>
+        <v>0.20750873584905652</v>
       </c>
     </row>
     <row r="90" spans="1:45" x14ac:dyDescent="0.5">
@@ -7935,13 +7935,13 @@
         <v>0</v>
       </c>
       <c r="AP90">
-        <v>8.9689371470437804E-2</v>
+        <v>8.9689371470437818E-2</v>
       </c>
       <c r="AQ90">
         <v>0.20697192630008165</v>
       </c>
       <c r="AR90">
-        <v>7.0370854944656405E-2</v>
+        <v>7.0370854944656419E-2</v>
       </c>
       <c r="AS90">
         <v>0.20179554539803135</v>
@@ -8054,7 +8054,7 @@
         <v>0</v>
       </c>
       <c r="AP91">
-        <v>8.8535242464194308E-2</v>
+        <v>8.8535242464194336E-2</v>
       </c>
       <c r="AQ91">
         <v>0.21354412756162663</v>
@@ -8179,13 +8179,13 @@
         <v>0</v>
       </c>
       <c r="AP92">
-        <v>0.11253011320754711</v>
+        <v>0.11253011320754709</v>
       </c>
       <c r="AQ92">
         <v>0.2130439898869009</v>
       </c>
       <c r="AR92">
-        <v>0.12253011320754706</v>
+        <v>0.12253011320754705</v>
       </c>
       <c r="AS92">
         <v>0.1957234818112121</v>
@@ -8298,13 +8298,13 @@
         <v>0</v>
       </c>
       <c r="AP93">
-        <v>0.1249875556434544</v>
+        <v>0.12498755564345439</v>
       </c>
       <c r="AQ93">
         <v>0.21441551297552461</v>
       </c>
       <c r="AR93">
-        <v>0.11007267077163976</v>
+        <v>0.11007267077163975</v>
       </c>
       <c r="AS93">
         <v>0.1943519587225884</v>
@@ -8414,13 +8414,13 @@
         <v>8.0030113207547104E-2</v>
       </c>
       <c r="AQ94">
-        <v>0.23913373584905637</v>
+        <v>0.23913373584905634</v>
       </c>
       <c r="AR94">
         <v>6.1280113207547102E-2</v>
       </c>
       <c r="AS94">
-        <v>0.23913373584905637</v>
+        <v>0.23913373584905634</v>
       </c>
     </row>
     <row r="95" spans="1:45" x14ac:dyDescent="0.5">
@@ -8527,13 +8527,13 @@
         <v>8.0030113207547104E-2</v>
       </c>
       <c r="AQ95">
-        <v>0.23913373584905656</v>
+        <v>0.23913373584905651</v>
       </c>
       <c r="AR95">
         <v>0.1175301132075471</v>
       </c>
       <c r="AS95">
-        <v>0.23913373584905656</v>
+        <v>0.23913373584905651</v>
       </c>
     </row>
     <row r="96" spans="1:45" x14ac:dyDescent="0.5">
@@ -9478,13 +9478,13 @@
         <v>0.21676071698113181</v>
       </c>
       <c r="AQ107">
-        <v>0.1764790448157911</v>
+        <v>0.17647904481579105</v>
       </c>
       <c r="AR107">
         <v>0.25426071698113184</v>
       </c>
       <c r="AS107">
-        <v>0.1764790448157911</v>
+        <v>0.17647904481579105</v>
       </c>
     </row>
     <row r="108" spans="1:45" s="4" customFormat="1" x14ac:dyDescent="0.5">
@@ -10468,10 +10468,10 @@
         <v>0</v>
       </c>
       <c r="AP119">
-        <v>0.34185913666902662</v>
+        <v>0.34185913666902673</v>
       </c>
       <c r="AQ119">
-        <v>0.13499630084857919</v>
+        <v>0.13499630084857916</v>
       </c>
       <c r="AR119">
         <v>0</v>
@@ -10756,10 +10756,10 @@
         <v>2</v>
       </c>
       <c r="O125">
-        <v>0.30460033668052133</v>
+        <v>0.30442814140648361</v>
       </c>
       <c r="P125">
-        <v>7.6355819300822123E-2</v>
+        <v>7.616736879291526E-2</v>
       </c>
       <c r="Q125">
         <v>0.28439264478139581</v>

</xml_diff>